<commit_message>
Actualizacion de archivos caracteristicas
</commit_message>
<xml_diff>
--- a/caracteristicas2.0/driveCARAC.xlsx
+++ b/caracteristicas2.0/driveCARAC.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\users\felipe\Mis Documentos\IABO_TENIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\IABO_DS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B1DFEE5-AB7A-4956-A35B-C7A10AD4779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dato" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,20 @@
     <sheet name="MIN" sheetId="5" r:id="rId5"/>
     <sheet name="MAX" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -32,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -530,48 +544,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -902,12 +916,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1">
@@ -53653,14 +53667,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F230"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217:XFD230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1">
@@ -59276,370 +59290,6 @@
       <c r="F216" s="1">
         <f>AVERAGE(dato!G2151:'dato'!G2160)</f>
         <v>-75.067138500000013</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6">
-      <c r="A217" s="1">
-        <f>AVERAGE(dato!B2161:'dato'!B2170)</f>
-        <v>-0.64279779999999997</v>
-      </c>
-      <c r="B217" s="1">
-        <f>AVERAGE(dato!C2161:'dato'!C2170)</f>
-        <v>0.15488279999999999</v>
-      </c>
-      <c r="C217" s="1">
-        <f>AVERAGE(dato!D2161:'dato'!D2170)</f>
-        <v>0.90578619999999999</v>
-      </c>
-      <c r="D217" s="1">
-        <f>AVERAGE(dato!E2161:'dato'!E2170)</f>
-        <v>6.1401367000000011</v>
-      </c>
-      <c r="E217" s="1">
-        <f>AVERAGE(dato!F2161:'dato'!F2170)</f>
-        <v>-24.829101599999994</v>
-      </c>
-      <c r="F217" s="1">
-        <f>AVERAGE(dato!G2161:'dato'!G2170)</f>
-        <v>-4.2236329999999995</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6">
-      <c r="A218" s="1">
-        <f>AVERAGE(dato!B2171:'dato'!B2180)</f>
-        <v>-0.69528810000000008</v>
-      </c>
-      <c r="B218" s="1">
-        <f>AVERAGE(dato!C2171:'dato'!C2180)</f>
-        <v>0.17473140000000004</v>
-      </c>
-      <c r="C218" s="1">
-        <f>AVERAGE(dato!D2171:'dato'!D2180)</f>
-        <v>0.92501220000000006</v>
-      </c>
-      <c r="D218" s="1">
-        <f>AVERAGE(dato!E2171:'dato'!E2180)</f>
-        <v>9.8022460999999996</v>
-      </c>
-      <c r="E218" s="1">
-        <f>AVERAGE(dato!F2171:'dato'!F2180)</f>
-        <v>22.698974700000001</v>
-      </c>
-      <c r="F218" s="1">
-        <f>AVERAGE(dato!G2171:'dato'!G2180)</f>
-        <v>-16.796875</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6">
-      <c r="A219" s="1">
-        <f>AVERAGE(dato!B2181:'dato'!B2190)</f>
-        <v>-2.9144899999999998</v>
-      </c>
-      <c r="B219" s="1">
-        <f>AVERAGE(dato!C2181:'dato'!C2190)</f>
-        <v>-1.1190673</v>
-      </c>
-      <c r="C219" s="1">
-        <f>AVERAGE(dato!D2181:'dato'!D2190)</f>
-        <v>3.2537598999999995</v>
-      </c>
-      <c r="D219" s="1">
-        <f>AVERAGE(dato!E2181:'dato'!E2190)</f>
-        <v>90.417480399999988</v>
-      </c>
-      <c r="E219" s="1">
-        <f>AVERAGE(dato!F2181:'dato'!F2190)</f>
-        <v>368.84155250000003</v>
-      </c>
-      <c r="F219" s="1">
-        <f>AVERAGE(dato!G2181:'dato'!G2190)</f>
-        <v>286.67602550000004</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6">
-      <c r="A220" s="1">
-        <f>AVERAGE(dato!B2191:'dato'!B2200)</f>
-        <v>-2.2370606000000004</v>
-      </c>
-      <c r="B220" s="1">
-        <f>AVERAGE(dato!C2191:'dato'!C2200)</f>
-        <v>1.5444947</v>
-      </c>
-      <c r="C220" s="1">
-        <f>AVERAGE(dato!D2191:'dato'!D2200)</f>
-        <v>-0.10029289999999998</v>
-      </c>
-      <c r="D220" s="1">
-        <f>AVERAGE(dato!E2191:'dato'!E2200)</f>
-        <v>123.09570320000003</v>
-      </c>
-      <c r="E220" s="1">
-        <f>AVERAGE(dato!F2191:'dato'!F2200)</f>
-        <v>236.46240240000006</v>
-      </c>
-      <c r="F220" s="1">
-        <f>AVERAGE(dato!G2191:'dato'!G2200)</f>
-        <v>284.0393067</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6">
-      <c r="A221" s="1">
-        <f>AVERAGE(dato!B2201:'dato'!B2210)</f>
-        <v>0.22548839999999998</v>
-      </c>
-      <c r="B221" s="1">
-        <f>AVERAGE(dato!C2201:'dato'!C2210)</f>
-        <v>1.1104492000000001</v>
-      </c>
-      <c r="C221" s="1">
-        <f>AVERAGE(dato!D2201:'dato'!D2210)</f>
-        <v>0.29447050000000002</v>
-      </c>
-      <c r="D221" s="1">
-        <f>AVERAGE(dato!E2201:'dato'!E2210)</f>
-        <v>13.732910100000002</v>
-      </c>
-      <c r="E221" s="1">
-        <f>AVERAGE(dato!F2201:'dato'!F2210)</f>
-        <v>-10.955810699999999</v>
-      </c>
-      <c r="F221" s="1">
-        <f>AVERAGE(dato!G2201:'dato'!G2210)</f>
-        <v>-26.684570199999996</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222" s="1">
-        <f>AVERAGE(dato!B2211:'dato'!B2220)</f>
-        <v>6.1181599999999989E-2</v>
-      </c>
-      <c r="B222" s="1">
-        <f>AVERAGE(dato!C2211:'dato'!C2220)</f>
-        <v>1.0289063000000001</v>
-      </c>
-      <c r="C222" s="1">
-        <f>AVERAGE(dato!D2211:'dato'!D2220)</f>
-        <v>0.25521240000000001</v>
-      </c>
-      <c r="D222" s="1">
-        <f>AVERAGE(dato!E2211:'dato'!E2220)</f>
-        <v>0.89111339999999972</v>
-      </c>
-      <c r="E222" s="1">
-        <f>AVERAGE(dato!F2211:'dato'!F2220)</f>
-        <v>-37.5</v>
-      </c>
-      <c r="F222" s="1">
-        <f>AVERAGE(dato!G2211:'dato'!G2220)</f>
-        <v>-56.335449000000004</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223" s="1">
-        <f>AVERAGE(dato!B2221:'dato'!B2230)</f>
-        <v>-4.1821299999999992E-2</v>
-      </c>
-      <c r="B223" s="1">
-        <f>AVERAGE(dato!C2221:'dato'!C2230)</f>
-        <v>0.7815917</v>
-      </c>
-      <c r="C223" s="1">
-        <f>AVERAGE(dato!D2221:'dato'!D2230)</f>
-        <v>0.42292479999999999</v>
-      </c>
-      <c r="D223" s="1">
-        <f>AVERAGE(dato!E2221:'dato'!E2230)</f>
-        <v>-81.146240300000002</v>
-      </c>
-      <c r="E223" s="1">
-        <f>AVERAGE(dato!F2221:'dato'!F2230)</f>
-        <v>-99.029540999999995</v>
-      </c>
-      <c r="F223" s="1">
-        <f>AVERAGE(dato!G2221:'dato'!G2230)</f>
-        <v>-209.75952160000003</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="A224" s="1">
-        <f>AVERAGE(dato!B2231:'dato'!B2240)</f>
-        <v>-0.45968010000000004</v>
-      </c>
-      <c r="B224" s="1">
-        <f>AVERAGE(dato!C2231:'dato'!C2240)</f>
-        <v>-0.26977540000000005</v>
-      </c>
-      <c r="C224" s="1">
-        <f>AVERAGE(dato!D2231:'dato'!D2240)</f>
-        <v>0.83107909999999996</v>
-      </c>
-      <c r="D224" s="1">
-        <f>AVERAGE(dato!E2231:'dato'!E2240)</f>
-        <v>-73.968505899999997</v>
-      </c>
-      <c r="E224" s="1">
-        <f>AVERAGE(dato!F2231:'dato'!F2240)</f>
-        <v>-188.3056641</v>
-      </c>
-      <c r="F224" s="1">
-        <f>AVERAGE(dato!G2231:'dato'!G2240)</f>
-        <v>-225.04272459999999</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="1">
-        <f>AVERAGE(dato!B2241:'dato'!B2250)</f>
-        <v>-0.79671639999999999</v>
-      </c>
-      <c r="B225" s="1">
-        <f>AVERAGE(dato!C2241:'dato'!C2250)</f>
-        <v>-2.56224E-2</v>
-      </c>
-      <c r="C225" s="1">
-        <f>AVERAGE(dato!D2241:'dato'!D2250)</f>
-        <v>1.3673097000000003</v>
-      </c>
-      <c r="D225" s="1">
-        <f>AVERAGE(dato!E2241:'dato'!E2250)</f>
-        <v>-66.375732400000004</v>
-      </c>
-      <c r="E225" s="1">
-        <f>AVERAGE(dato!F2241:'dato'!F2250)</f>
-        <v>-140.6799317</v>
-      </c>
-      <c r="F225" s="1">
-        <f>AVERAGE(dato!G2241:'dato'!G2250)</f>
-        <v>-82.208251900000008</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="1">
-        <f>AVERAGE(dato!B2251:'dato'!B2260)</f>
-        <v>-0.67012950000000004</v>
-      </c>
-      <c r="B226" s="1">
-        <f>AVERAGE(dato!C2251:'dato'!C2260)</f>
-        <v>0.17601320000000001</v>
-      </c>
-      <c r="C226" s="1">
-        <f>AVERAGE(dato!D2251:'dato'!D2260)</f>
-        <v>1.0311889999999999</v>
-      </c>
-      <c r="D226" s="1">
-        <f>AVERAGE(dato!E2251:'dato'!E2260)</f>
-        <v>1.8920896000000003</v>
-      </c>
-      <c r="E226" s="1">
-        <f>AVERAGE(dato!F2251:'dato'!F2260)</f>
-        <v>-56.689453200000003</v>
-      </c>
-      <c r="F226" s="1">
-        <f>AVERAGE(dato!G2251:'dato'!G2260)</f>
-        <v>-39.294433400000003</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6">
-      <c r="A227" s="1">
-        <f>AVERAGE(dato!B2261:'dato'!B2270)</f>
-        <v>-0.69969480000000006</v>
-      </c>
-      <c r="B227" s="1">
-        <f>AVERAGE(dato!C2261:'dato'!C2270)</f>
-        <v>0.32744129999999999</v>
-      </c>
-      <c r="C227" s="1">
-        <f>AVERAGE(dato!D2261:'dato'!D2270)</f>
-        <v>0.64384770000000002</v>
-      </c>
-      <c r="D227" s="1">
-        <f>AVERAGE(dato!E2261:'dato'!E2270)</f>
-        <v>19.500732599999999</v>
-      </c>
-      <c r="E227" s="1">
-        <f>AVERAGE(dato!F2261:'dato'!F2270)</f>
-        <v>-18.676757700000003</v>
-      </c>
-      <c r="F227" s="1">
-        <f>AVERAGE(dato!G2261:'dato'!G2270)</f>
-        <v>-23.321533199999998</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6">
-      <c r="A228" s="1">
-        <f>AVERAGE(dato!B2271:'dato'!B2280)</f>
-        <v>-0.73383799999999999</v>
-      </c>
-      <c r="B228" s="1">
-        <f>AVERAGE(dato!C2271:'dato'!C2280)</f>
-        <v>0.24840100000000001</v>
-      </c>
-      <c r="C228" s="1">
-        <f>AVERAGE(dato!D2271:'dato'!D2280)</f>
-        <v>0.87318109999999982</v>
-      </c>
-      <c r="D228" s="1">
-        <f>AVERAGE(dato!E2271:'dato'!E2280)</f>
-        <v>12.109374900000001</v>
-      </c>
-      <c r="E228" s="1">
-        <f>AVERAGE(dato!F2271:'dato'!F2280)</f>
-        <v>17.504882900000002</v>
-      </c>
-      <c r="F228" s="1">
-        <f>AVERAGE(dato!G2271:'dato'!G2280)</f>
-        <v>-2.5207519000000005</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6">
-      <c r="A229" s="1">
-        <f>AVERAGE(dato!B2281:'dato'!B2290)</f>
-        <v>-2.6585327999999997</v>
-      </c>
-      <c r="B229" s="1">
-        <f>AVERAGE(dato!C2281:'dato'!C2290)</f>
-        <v>-1.0532958999999997</v>
-      </c>
-      <c r="C229" s="1">
-        <f>AVERAGE(dato!D2281:'dato'!D2290)</f>
-        <v>3.1993408999999997</v>
-      </c>
-      <c r="D229" s="1">
-        <f>AVERAGE(dato!E2281:'dato'!E2290)</f>
-        <v>80.596923799999999</v>
-      </c>
-      <c r="E229" s="1">
-        <f>AVERAGE(dato!F2281:'dato'!F2290)</f>
-        <v>279.05883800000004</v>
-      </c>
-      <c r="F229" s="1">
-        <f>AVERAGE(dato!G2281:'dato'!G2290)</f>
-        <v>235.98022469999995</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6">
-      <c r="A230" s="1">
-        <f>AVERAGE(dato!B2291:'dato'!B2300)</f>
-        <v>-3.9995120000000006</v>
-      </c>
-      <c r="B230" s="1">
-        <f>AVERAGE(dato!C2291:'dato'!C2300)</f>
-        <v>2.0141333333333306E-2</v>
-      </c>
-      <c r="C230" s="1">
-        <f>AVERAGE(dato!D2291:'dato'!D2300)</f>
-        <v>0.74658200000000008</v>
-      </c>
-      <c r="D230" s="1">
-        <f>AVERAGE(dato!E2291:'dato'!E2300)</f>
-        <v>191.85384133333332</v>
-      </c>
-      <c r="E230" s="1">
-        <f>AVERAGE(dato!F2291:'dato'!F2300)</f>
-        <v>657.28759766666667</v>
-      </c>
-      <c r="F230" s="1">
-        <f>AVERAGE(dato!G2291:'dato'!G2300)</f>
-        <v>644.42952466666657</v>
       </c>
     </row>
   </sheetData>
@@ -59648,14 +59298,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F230"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F230"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217:XFD230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1">
@@ -65271,370 +64921,6 @@
       <c r="F216" s="1">
         <f>_xlfn.VAR.S(dato!G2151:'dato'!G2160)</f>
         <v>688.18400631194368</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6">
-      <c r="A217" s="1">
-        <f>_xlfn.VAR.S(dato!B2161:'dato'!B2170)</f>
-        <v>4.3096264995555597E-4</v>
-      </c>
-      <c r="B217" s="1">
-        <f>_xlfn.VAR.S(dato!C2161:'dato'!C2170)</f>
-        <v>1.308941186484445E-2</v>
-      </c>
-      <c r="C217" s="1">
-        <f>_xlfn.VAR.S(dato!D2161:'dato'!D2170)</f>
-        <v>2.5781161411510805E-2</v>
-      </c>
-      <c r="D217" s="1">
-        <f>_xlfn.VAR.S(dato!E2161:'dato'!E2170)</f>
-        <v>99.661614682345999</v>
-      </c>
-      <c r="E217" s="1">
-        <f>_xlfn.VAR.S(dato!F2161:'dato'!F2170)</f>
-        <v>751.95133816375767</v>
-      </c>
-      <c r="F217" s="1">
-        <f>_xlfn.VAR.S(dato!G2161:'dato'!G2170)</f>
-        <v>83.726977431403327</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6">
-      <c r="A218" s="1">
-        <f>_xlfn.VAR.S(dato!B2171:'dato'!B2180)</f>
-        <v>7.1225092574333081E-3</v>
-      </c>
-      <c r="B218" s="1">
-        <f>_xlfn.VAR.S(dato!C2171:'dato'!C2180)</f>
-        <v>2.3708131945822206E-2</v>
-      </c>
-      <c r="C218" s="1">
-        <f>_xlfn.VAR.S(dato!D2171:'dato'!D2180)</f>
-        <v>0.13853512655684419</v>
-      </c>
-      <c r="D218" s="1">
-        <f>_xlfn.VAR.S(dato!E2171:'dato'!E2180)</f>
-        <v>42.911372886149238</v>
-      </c>
-      <c r="E218" s="1">
-        <f>_xlfn.VAR.S(dato!F2171:'dato'!F2180)</f>
-        <v>124.30585857482482</v>
-      </c>
-      <c r="F218" s="1">
-        <f>_xlfn.VAR.S(dato!G2171:'dato'!G2180)</f>
-        <v>100.9444385901558</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6">
-      <c r="A219" s="1">
-        <f>_xlfn.VAR.S(dato!B2181:'dato'!B2190)</f>
-        <v>1.7905523954571154</v>
-      </c>
-      <c r="B219" s="1">
-        <f>_xlfn.VAR.S(dato!C2181:'dato'!C2190)</f>
-        <v>1.1328770258600114</v>
-      </c>
-      <c r="C219" s="1">
-        <f>_xlfn.VAR.S(dato!D2181:'dato'!D2190)</f>
-        <v>1.0117514793734397</v>
-      </c>
-      <c r="D219" s="1">
-        <f>_xlfn.VAR.S(dato!E2181:'dato'!E2190)</f>
-        <v>3092.1277241324537</v>
-      </c>
-      <c r="E219" s="1">
-        <f>_xlfn.VAR.S(dato!F2181:'dato'!F2190)</f>
-        <v>91855.44524807384</v>
-      </c>
-      <c r="F219" s="1">
-        <f>_xlfn.VAR.S(dato!G2181:'dato'!G2190)</f>
-        <v>69592.022578318996</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6">
-      <c r="A220" s="1">
-        <f>_xlfn.VAR.S(dato!B2191:'dato'!B2200)</f>
-        <v>2.1379368674395973</v>
-      </c>
-      <c r="B220" s="1">
-        <f>_xlfn.VAR.S(dato!C2191:'dato'!C2200)</f>
-        <v>1.2390835268124551</v>
-      </c>
-      <c r="C220" s="1">
-        <f>_xlfn.VAR.S(dato!D2191:'dato'!D2200)</f>
-        <v>0.19662839705832219</v>
-      </c>
-      <c r="D220" s="1">
-        <f>_xlfn.VAR.S(dato!E2191:'dato'!E2200)</f>
-        <v>6190.4008355762862</v>
-      </c>
-      <c r="E220" s="1">
-        <f>_xlfn.VAR.S(dato!F2191:'dato'!F2200)</f>
-        <v>30453.926859740917</v>
-      </c>
-      <c r="F220" s="1">
-        <f>_xlfn.VAR.S(dato!G2191:'dato'!G2200)</f>
-        <v>41230.561889070319</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6">
-      <c r="A221" s="1">
-        <f>_xlfn.VAR.S(dato!B2201:'dato'!B2210)</f>
-        <v>9.6260637984889111E-3</v>
-      </c>
-      <c r="B221" s="1">
-        <f>_xlfn.VAR.S(dato!C2201:'dato'!C2210)</f>
-        <v>9.5495098199955483E-2</v>
-      </c>
-      <c r="C221" s="1">
-        <f>_xlfn.VAR.S(dato!D2201:'dato'!D2210)</f>
-        <v>9.2977779610277742E-2</v>
-      </c>
-      <c r="D221" s="1">
-        <f>_xlfn.VAR.S(dato!E2201:'dato'!E2210)</f>
-        <v>482.2636651310392</v>
-      </c>
-      <c r="E221" s="1">
-        <f>_xlfn.VAR.S(dato!F2201:'dato'!F2210)</f>
-        <v>355.36309524483153</v>
-      </c>
-      <c r="F221" s="1">
-        <f>_xlfn.VAR.S(dato!G2201:'dato'!G2210)</f>
-        <v>993.13325750020385</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222" s="1">
-        <f>_xlfn.VAR.S(dato!B2211:'dato'!B2220)</f>
-        <v>1.5191986229333354E-3</v>
-      </c>
-      <c r="B222" s="1">
-        <f>_xlfn.VAR.S(dato!C2211:'dato'!C2220)</f>
-        <v>6.5575241134444408E-4</v>
-      </c>
-      <c r="C222" s="1">
-        <f>_xlfn.VAR.S(dato!D2211:'dato'!D2220)</f>
-        <v>2.1878280589155554E-2</v>
-      </c>
-      <c r="D222" s="1">
-        <f>_xlfn.VAR.S(dato!E2211:'dato'!E2220)</f>
-        <v>298.79907999894897</v>
-      </c>
-      <c r="E222" s="1">
-        <f>_xlfn.VAR.S(dato!F2211:'dato'!F2220)</f>
-        <v>319.65159915881668</v>
-      </c>
-      <c r="F222" s="1">
-        <f>_xlfn.VAR.S(dato!G2211:'dato'!G2220)</f>
-        <v>1136.8360854678674</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223" s="1">
-        <f>_xlfn.VAR.S(dato!B2221:'dato'!B2230)</f>
-        <v>1.1158159182333342E-3</v>
-      </c>
-      <c r="B223" s="1">
-        <f>_xlfn.VAR.S(dato!C2221:'dato'!C2230)</f>
-        <v>8.59191090909001E-2</v>
-      </c>
-      <c r="C223" s="1">
-        <f>_xlfn.VAR.S(dato!D2221:'dato'!D2230)</f>
-        <v>2.8625953243999933E-3</v>
-      </c>
-      <c r="D223" s="1">
-        <f>_xlfn.VAR.S(dato!E2221:'dato'!E2230)</f>
-        <v>1131.1117575758819</v>
-      </c>
-      <c r="E223" s="1">
-        <f>_xlfn.VAR.S(dato!F2221:'dato'!F2230)</f>
-        <v>2565.6035039442941</v>
-      </c>
-      <c r="F223" s="1">
-        <f>_xlfn.VAR.S(dato!G2221:'dato'!G2230)</f>
-        <v>2163.2926644046934</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="A224" s="1">
-        <f>_xlfn.VAR.S(dato!B2231:'dato'!B2240)</f>
-        <v>4.4642315010766681E-2</v>
-      </c>
-      <c r="B224" s="1">
-        <f>_xlfn.VAR.S(dato!C2231:'dato'!C2240)</f>
-        <v>7.8209007356488877E-2</v>
-      </c>
-      <c r="C224" s="1">
-        <f>_xlfn.VAR.S(dato!D2231:'dato'!D2240)</f>
-        <v>4.5045557734988764E-2</v>
-      </c>
-      <c r="D224" s="1">
-        <f>_xlfn.VAR.S(dato!E2231:'dato'!E2240)</f>
-        <v>530.38236988430026</v>
-      </c>
-      <c r="E224" s="1">
-        <f>_xlfn.VAR.S(dato!F2231:'dato'!F2240)</f>
-        <v>348.69528492253636</v>
-      </c>
-      <c r="F224" s="1">
-        <f>_xlfn.VAR.S(dato!G2231:'dato'!G2240)</f>
-        <v>2734.831187317568</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="1">
-        <f>_xlfn.VAR.S(dato!B2241:'dato'!B2250)</f>
-        <v>3.8264778973777797E-3</v>
-      </c>
-      <c r="B225" s="1">
-        <f>_xlfn.VAR.S(dato!C2241:'dato'!C2250)</f>
-        <v>2.6462530189155557E-2</v>
-      </c>
-      <c r="C225" s="1">
-        <f>_xlfn.VAR.S(dato!D2241:'dato'!D2250)</f>
-        <v>2.4245429660455089E-2</v>
-      </c>
-      <c r="D225" s="1">
-        <f>_xlfn.VAR.S(dato!E2241:'dato'!E2250)</f>
-        <v>1260.1053153528644</v>
-      </c>
-      <c r="E225" s="1">
-        <f>_xlfn.VAR.S(dato!F2241:'dato'!F2250)</f>
-        <v>1340.6296904780741</v>
-      </c>
-      <c r="F225" s="1">
-        <f>_xlfn.VAR.S(dato!G2241:'dato'!G2250)</f>
-        <v>858.64334999786092</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="1">
-        <f>_xlfn.VAR.S(dato!B2251:'dato'!B2260)</f>
-        <v>1.4028088298333342E-3</v>
-      </c>
-      <c r="B226" s="1">
-        <f>_xlfn.VAR.S(dato!C2251:'dato'!C2260)</f>
-        <v>3.0178720352888907E-3</v>
-      </c>
-      <c r="C226" s="1">
-        <f>_xlfn.VAR.S(dato!D2251:'dato'!D2260)</f>
-        <v>4.2080548141555402E-2</v>
-      </c>
-      <c r="D226" s="1">
-        <f>_xlfn.VAR.S(dato!E2251:'dato'!E2260)</f>
-        <v>92.500613702986044</v>
-      </c>
-      <c r="E226" s="1">
-        <f>_xlfn.VAR.S(dato!F2251:'dato'!F2260)</f>
-        <v>636.33819576805968</v>
-      </c>
-      <c r="F226" s="1">
-        <f>_xlfn.VAR.S(dato!G2251:'dato'!G2260)</f>
-        <v>141.52940733532321</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6">
-      <c r="A227" s="1">
-        <f>_xlfn.VAR.S(dato!B2261:'dato'!B2270)</f>
-        <v>3.0066503306666717E-4</v>
-      </c>
-      <c r="B227" s="1">
-        <f>_xlfn.VAR.S(dato!C2261:'dato'!C2270)</f>
-        <v>3.5379054720111234E-3</v>
-      </c>
-      <c r="C227" s="1">
-        <f>_xlfn.VAR.S(dato!D2261:'dato'!D2270)</f>
-        <v>2.9312727546777786E-3</v>
-      </c>
-      <c r="D227" s="1">
-        <f>_xlfn.VAR.S(dato!E2261:'dato'!E2270)</f>
-        <v>37.42612779818657</v>
-      </c>
-      <c r="E227" s="1">
-        <f>_xlfn.VAR.S(dato!F2261:'dato'!F2270)</f>
-        <v>49.039723267449318</v>
-      </c>
-      <c r="F227" s="1">
-        <f>_xlfn.VAR.S(dato!G2261:'dato'!G2270)</f>
-        <v>35.807865268855899</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6">
-      <c r="A228" s="1">
-        <f>_xlfn.VAR.S(dato!B2271:'dato'!B2280)</f>
-        <v>1.1914494717777637E-2</v>
-      </c>
-      <c r="B228" s="1">
-        <f>_xlfn.VAR.S(dato!C2271:'dato'!C2280)</f>
-        <v>2.0813195986666658E-2</v>
-      </c>
-      <c r="C228" s="1">
-        <f>_xlfn.VAR.S(dato!D2271:'dato'!D2280)</f>
-        <v>6.3774452334766918E-2</v>
-      </c>
-      <c r="D228" s="1">
-        <f>_xlfn.VAR.S(dato!E2271:'dato'!E2280)</f>
-        <v>8.5526047654893773</v>
-      </c>
-      <c r="E228" s="1">
-        <f>_xlfn.VAR.S(dato!F2271:'dato'!F2280)</f>
-        <v>300.8045997155931</v>
-      </c>
-      <c r="F228" s="1">
-        <f>_xlfn.VAR.S(dato!G2271:'dato'!G2280)</f>
-        <v>120.7499457704121</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6">
-      <c r="A229" s="1">
-        <f>_xlfn.VAR.S(dato!B2281:'dato'!B2290)</f>
-        <v>1.5889516852746257</v>
-      </c>
-      <c r="B229" s="1">
-        <f>_xlfn.VAR.S(dato!C2281:'dato'!C2290)</f>
-        <v>1.0234904860556564</v>
-      </c>
-      <c r="C229" s="1">
-        <f>_xlfn.VAR.S(dato!D2281:'dato'!D2290)</f>
-        <v>0.91836650227366101</v>
-      </c>
-      <c r="D229" s="1">
-        <f>_xlfn.VAR.S(dato!E2281:'dato'!E2290)</f>
-        <v>6697.6392153751585</v>
-      </c>
-      <c r="E229" s="1">
-        <f>_xlfn.VAR.S(dato!F2281:'dato'!F2290)</f>
-        <v>54737.429982072958</v>
-      </c>
-      <c r="F229" s="1">
-        <f>_xlfn.VAR.S(dato!G2281:'dato'!G2290)</f>
-        <v>56693.687287244858</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6">
-      <c r="A230" s="1">
-        <f>_xlfn.VAR.S(dato!B2291:'dato'!B2300)</f>
-        <v>2.9582283945787943E-31</v>
-      </c>
-      <c r="B230" s="1">
-        <f>_xlfn.VAR.S(dato!C2291:'dato'!C2300)</f>
-        <v>0.2355717000723333</v>
-      </c>
-      <c r="C230" s="1">
-        <f>_xlfn.VAR.S(dato!D2291:'dato'!D2300)</f>
-        <v>2.1865294965239999</v>
-      </c>
-      <c r="D230" s="1">
-        <f>_xlfn.VAR.S(dato!E2291:'dato'!E2300)</f>
-        <v>4249.1567393258447</v>
-      </c>
-      <c r="E230" s="1">
-        <f>_xlfn.VAR.S(dato!F2291:'dato'!F2300)</f>
-        <v>26790.198043741286</v>
-      </c>
-      <c r="F230" s="1">
-        <f>_xlfn.VAR.S(dato!G2291:'dato'!G2300)</f>
-        <v>4390.3638448562615</v>
       </c>
     </row>
   </sheetData>
@@ -65643,14 +64929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F230"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217:XFD230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1">
@@ -71266,370 +70552,6 @@
       <c r="F216" s="1">
         <f>SUMSQ(dato!G2151:'dato'!G2160)</f>
         <v>62544.408882589334</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6">
-      <c r="A217" s="1">
-        <f>SUMSQ(dato!B2161:'dato'!B2170)</f>
-        <v>4.1357687806980001</v>
-      </c>
-      <c r="B217" s="1">
-        <f>SUMSQ(dato!C2161:'dato'!C2170)</f>
-        <v>0.35769152414200001</v>
-      </c>
-      <c r="C217" s="1">
-        <f>SUMSQ(dato!D2161:'dato'!D2170)</f>
-        <v>8.4365168538079978</v>
-      </c>
-      <c r="D217" s="1">
-        <f>SUMSQ(dato!E2161:'dato'!E2170)</f>
-        <v>1273.967319087983</v>
-      </c>
-      <c r="E217" s="1">
-        <f>SUMSQ(dato!F2161:'dato'!F2170)</f>
-        <v>12932.404906105043</v>
-      </c>
-      <c r="F217" s="1">
-        <f>SUMSQ(dato!G2161:'dato'!G2170)</f>
-        <v>931.93355406951991</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6">
-      <c r="A218" s="1">
-        <f>SUMSQ(dato!B2171:'dato'!B2180)</f>
-        <v>4.8983580033330005</v>
-      </c>
-      <c r="B218" s="1">
-        <f>SUMSQ(dato!C2171:'dato'!C2180)</f>
-        <v>0.51868380897199995</v>
-      </c>
-      <c r="C218" s="1">
-        <f>SUMSQ(dato!D2171:'dato'!D2180)</f>
-        <v>9.8032918405</v>
-      </c>
-      <c r="D218" s="1">
-        <f>SUMSQ(dato!E2171:'dato'!E2180)</f>
-        <v>1347.0426420249951</v>
-      </c>
-      <c r="E218" s="1">
-        <f>SUMSQ(dato!F2171:'dato'!F2180)</f>
-        <v>6271.187251485826</v>
-      </c>
-      <c r="F218" s="1">
-        <f>SUMSQ(dato!G2171:'dato'!G2180)</f>
-        <v>3729.8500449676521</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6">
-      <c r="A219" s="1">
-        <f>SUMSQ(dato!B2181:'dato'!B2190)</f>
-        <v>101.05749116011403</v>
-      </c>
-      <c r="B219" s="1">
-        <f>SUMSQ(dato!C2181:'dato'!C2190)</f>
-        <v>22.719009452033003</v>
-      </c>
-      <c r="C219" s="1">
-        <f>SUMSQ(dato!D2181:'dato'!D2190)</f>
-        <v>114.97529818284102</v>
-      </c>
-      <c r="D219" s="1">
-        <f>SUMSQ(dato!E2181:'dato'!E2190)</f>
-        <v>109582.35713603591</v>
-      </c>
-      <c r="E219" s="1">
-        <f>SUMSQ(dato!F2181:'dato'!F2190)</f>
-        <v>2187139.9157387675</v>
-      </c>
-      <c r="F219" s="1">
-        <f>SUMSQ(dato!G2181:'dato'!G2190)</f>
-        <v>1448159.6391696376</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6">
-      <c r="A220" s="1">
-        <f>SUMSQ(dato!B2191:'dato'!B2200)</f>
-        <v>69.28583308767999</v>
-      </c>
-      <c r="B220" s="1">
-        <f>SUMSQ(dato!C2191:'dato'!C2200)</f>
-        <v>35.006390524592994</v>
-      </c>
-      <c r="C220" s="1">
-        <f>SUMSQ(dato!D2191:'dato'!D2200)</f>
-        <v>1.8702422314289997</v>
-      </c>
-      <c r="D220" s="1">
-        <f>SUMSQ(dato!E2191:'dato'!E2200)</f>
-        <v>207239.12898321153</v>
-      </c>
-      <c r="E220" s="1">
-        <f>SUMSQ(dato!F2191:'dato'!F2200)</f>
-        <v>833230.01922546374</v>
-      </c>
-      <c r="F220" s="1">
-        <f>SUMSQ(dato!G2191:'dato'!G2200)</f>
-        <v>1177858.3345077995</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6">
-      <c r="A221" s="1">
-        <f>SUMSQ(dato!B2201:'dato'!B2210)</f>
-        <v>0.59508475953200002</v>
-      </c>
-      <c r="B221" s="1">
-        <f>SUMSQ(dato!C2201:'dato'!C2210)</f>
-        <v>13.190430141605999</v>
-      </c>
-      <c r="C221" s="1">
-        <f>SUMSQ(dato!D2201:'dato'!D2210)</f>
-        <v>1.7039287701949999</v>
-      </c>
-      <c r="D221" s="1">
-        <f>SUMSQ(dato!E2201:'dato'!E2210)</f>
-        <v>6226.3011843261729</v>
-      </c>
-      <c r="E221" s="1">
-        <f>SUMSQ(dato!F2201:'dato'!F2210)</f>
-        <v>4398.5657381458286</v>
-      </c>
-      <c r="F221" s="1">
-        <f>SUMSQ(dato!G2201:'dato'!G2210)</f>
-        <v>16058.862185089112</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222" s="1">
-        <f>SUMSQ(dato!B2211:'dato'!B2220)</f>
-        <v>5.1104669392000007E-2</v>
-      </c>
-      <c r="B222" s="1">
-        <f>SUMSQ(dato!C2211:'dato'!C2220)</f>
-        <v>10.592383513499</v>
-      </c>
-      <c r="C222" s="1">
-        <f>SUMSQ(dato!D2211:'dato'!D2220)</f>
-        <v>0.84823821643999997</v>
-      </c>
-      <c r="D222" s="1">
-        <f>SUMSQ(dato!E2211:'dato'!E2220)</f>
-        <v>2697.1325509071362</v>
-      </c>
-      <c r="E222" s="1">
-        <f>SUMSQ(dato!F2211:'dato'!F2220)</f>
-        <v>16939.36439242935</v>
-      </c>
-      <c r="F222" s="1">
-        <f>SUMSQ(dato!G2211:'dato'!G2220)</f>
-        <v>41968.352909526824</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223" s="1">
-        <f>SUMSQ(dato!B2221:'dato'!B2230)</f>
-        <v>2.7532554601000004E-2</v>
-      </c>
-      <c r="B223" s="1">
-        <f>SUMSQ(dato!C2221:'dato'!C2230)</f>
-        <v>6.8821278369070003</v>
-      </c>
-      <c r="C223" s="1">
-        <f>SUMSQ(dato!D2221:'dato'!D2230)</f>
-        <v>1.8144172224699999</v>
-      </c>
-      <c r="D223" s="1">
-        <f>SUMSQ(dato!E2221:'dato'!E2230)</f>
-        <v>76027.128966436387</v>
-      </c>
-      <c r="E223" s="1">
-        <f>SUMSQ(dato!F2221:'dato'!F2230)</f>
-        <v>121158.93144220544</v>
-      </c>
-      <c r="F223" s="1">
-        <f>SUMSQ(dato!G2221:'dato'!G2230)</f>
-        <v>459460.20299825096</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="A224" s="1">
-        <f>SUMSQ(dato!B2231:'dato'!B2240)</f>
-        <v>2.5148387784569999</v>
-      </c>
-      <c r="B224" s="1">
-        <f>SUMSQ(dato!C2231:'dato'!C2240)</f>
-        <v>1.4316687306600002</v>
-      </c>
-      <c r="C224" s="1">
-        <f>SUMSQ(dato!D2231:'dato'!D2240)</f>
-        <v>7.3123347241829988</v>
-      </c>
-      <c r="D224" s="1">
-        <f>SUMSQ(dato!E2231:'dato'!E2240)</f>
-        <v>59486.83997974205</v>
-      </c>
-      <c r="E224" s="1">
-        <f>SUMSQ(dato!F2231:'dato'!F2240)</f>
-        <v>357728.48888572311</v>
-      </c>
-      <c r="F224" s="1">
-        <f>SUMSQ(dato!G2231:'dato'!G2240)</f>
-        <v>531055.75963977247</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="1">
-        <f>SUMSQ(dato!B2241:'dato'!B2250)</f>
-        <v>6.3820085213660001</v>
-      </c>
-      <c r="B225" s="1">
-        <f>SUMSQ(dato!C2241:'dato'!C2250)</f>
-        <v>0.24472784552000001</v>
-      </c>
-      <c r="C225" s="1">
-        <f>SUMSQ(dato!D2241:'dato'!D2250)</f>
-        <v>18.913567024085001</v>
-      </c>
-      <c r="D225" s="1">
-        <f>SUMSQ(dato!E2241:'dato'!E2250)</f>
-        <v>55398.32635453988</v>
-      </c>
-      <c r="E225" s="1">
-        <f>SUMSQ(dato!F2241:'dato'!F2250)</f>
-        <v>209974.09904546931</v>
-      </c>
-      <c r="F225" s="1">
-        <f>SUMSQ(dato!G2241:'dato'!G2250)</f>
-        <v>75309.756954519282</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="1">
-        <f>SUMSQ(dato!B2251:'dato'!B2260)</f>
-        <v>4.5033607471710004</v>
-      </c>
-      <c r="B226" s="1">
-        <f>SUMSQ(dato!C2251:'dato'!C2260)</f>
-        <v>0.33696731406000002</v>
-      </c>
-      <c r="C226" s="1">
-        <f>SUMSQ(dato!D2251:'dato'!D2260)</f>
-        <v>11.012232470483998</v>
-      </c>
-      <c r="D226" s="1">
-        <f>SUMSQ(dato!E2251:'dato'!E2260)</f>
-        <v>868.30555387115601</v>
-      </c>
-      <c r="E226" s="1">
-        <f>SUMSQ(dato!F2251:'dato'!F2260)</f>
-        <v>37863.984803062442</v>
-      </c>
-      <c r="F226" s="1">
-        <f>SUMSQ(dato!G2251:'dato'!G2260)</f>
-        <v>16714.289628288268</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6">
-      <c r="A227" s="1">
-        <f>SUMSQ(dato!B2261:'dato'!B2270)</f>
-        <v>4.8984341167679997</v>
-      </c>
-      <c r="B227" s="1">
-        <f>SUMSQ(dato!C2261:'dato'!C2270)</f>
-        <v>1.1040191987050001</v>
-      </c>
-      <c r="C227" s="1">
-        <f>SUMSQ(dato!D2261:'dato'!D2270)</f>
-        <v>4.1717800627449995</v>
-      </c>
-      <c r="D227" s="1">
-        <f>SUMSQ(dato!E2261:'dato'!E2270)</f>
-        <v>4139.6208695507057</v>
-      </c>
-      <c r="E227" s="1">
-        <f>SUMSQ(dato!F2261:'dato'!F2270)</f>
-        <v>3929.5702912521374</v>
-      </c>
-      <c r="F227" s="1">
-        <f>SUMSQ(dato!G2261:'dato'!G2270)</f>
-        <v>5761.2098954067251</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6">
-      <c r="A228" s="1">
-        <f>SUMSQ(dato!B2271:'dato'!B2280)</f>
-        <v>5.4924125548999987</v>
-      </c>
-      <c r="B228" s="1">
-        <f>SUMSQ(dato!C2271:'dato'!C2280)</f>
-        <v>0.80434933188999991</v>
-      </c>
-      <c r="C228" s="1">
-        <f>SUMSQ(dato!D2271:'dato'!D2280)</f>
-        <v>8.1984224049849992</v>
-      </c>
-      <c r="D228" s="1">
-        <f>SUMSQ(dato!E2271:'dato'!E2280)</f>
-        <v>1543.3430475769046</v>
-      </c>
-      <c r="E228" s="1">
-        <f>SUMSQ(dato!F2271:'dato'!F2280)</f>
-        <v>5771.4506508674622</v>
-      </c>
-      <c r="F228" s="1">
-        <f>SUMSQ(dato!G2271:'dato'!G2280)</f>
-        <v>1150.291413347245</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6">
-      <c r="A229" s="1">
-        <f>SUMSQ(dato!B2281:'dato'!B2290)</f>
-        <v>84.978531654230011</v>
-      </c>
-      <c r="B229" s="1">
-        <f>SUMSQ(dato!C2281:'dato'!C2290)</f>
-        <v>20.305736904069004</v>
-      </c>
-      <c r="C229" s="1">
-        <f>SUMSQ(dato!D2281:'dato'!D2290)</f>
-        <v>110.62312046459103</v>
-      </c>
-      <c r="D229" s="1">
-        <f>SUMSQ(dato!E2281:'dato'!E2290)</f>
-        <v>125237.39419860649</v>
-      </c>
-      <c r="E229" s="1">
-        <f>SUMSQ(dato!F2281:'dato'!F2290)</f>
-        <v>1271375.2204977591</v>
-      </c>
-      <c r="F229" s="1">
-        <f>SUMSQ(dato!G2281:'dato'!G2290)</f>
-        <v>1067109.8500798284</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6">
-      <c r="A230" s="1">
-        <f>SUMSQ(dato!B2291:'dato'!B2300)</f>
-        <v>47.988288714432002</v>
-      </c>
-      <c r="B230" s="1">
-        <f>SUMSQ(dato!C2291:'dato'!C2300)</f>
-        <v>0.47236042006999995</v>
-      </c>
-      <c r="C230" s="1">
-        <f>SUMSQ(dato!D2291:'dato'!D2300)</f>
-        <v>6.0452130412200002</v>
-      </c>
-      <c r="D230" s="1">
-        <f>SUMSQ(dato!E2291:'dato'!E2300)</f>
-        <v>118922.0027817192</v>
-      </c>
-      <c r="E230" s="1">
-        <f>SUMSQ(dato!F2291:'dato'!F2300)</f>
-        <v>1349661.3542267361</v>
-      </c>
-      <c r="F230" s="1">
-        <f>SUMSQ(dato!G2291:'dato'!G2300)</f>
-        <v>1254648.9644760303</v>
       </c>
     </row>
   </sheetData>
@@ -71638,14 +70560,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F230"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F230"/>
+    <sheetView topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217:XFD230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1">
@@ -77261,370 +76183,6 @@
       <c r="F216" s="1">
         <f>MIN(dato!G2151:'dato'!G2160)</f>
         <v>-100.95214799999999</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6">
-      <c r="A217" s="1">
-        <f>MIN(dato!B2161:'dato'!B2170)</f>
-        <v>-0.68335000000000001</v>
-      </c>
-      <c r="B217" s="1">
-        <f>MIN(dato!C2161:'dato'!C2170)</f>
-        <v>-2.3560000000000001E-2</v>
-      </c>
-      <c r="C217" s="1">
-        <f>MIN(dato!D2161:'dato'!D2170)</f>
-        <v>0.67382799999999998</v>
-      </c>
-      <c r="D217" s="1">
-        <f>MIN(dato!E2161:'dato'!E2170)</f>
-        <v>-7.0800780000000003</v>
-      </c>
-      <c r="E217" s="1">
-        <f>MIN(dato!F2161:'dato'!F2170)</f>
-        <v>-69.946288999999993</v>
-      </c>
-      <c r="F217" s="1">
-        <f>MIN(dato!G2161:'dato'!G2170)</f>
-        <v>-16.662597999999999</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6">
-      <c r="A218" s="1">
-        <f>MIN(dato!B2171:'dato'!B2180)</f>
-        <v>-0.852051</v>
-      </c>
-      <c r="B218" s="1">
-        <f>MIN(dato!C2171:'dato'!C2180)</f>
-        <v>-4.8584000000000002E-2</v>
-      </c>
-      <c r="C218" s="1">
-        <f>MIN(dato!D2171:'dato'!D2180)</f>
-        <v>0.60339399999999999</v>
-      </c>
-      <c r="D218" s="1">
-        <f>MIN(dato!E2171:'dato'!E2180)</f>
-        <v>3.2348629999999998</v>
-      </c>
-      <c r="E218" s="1">
-        <f>MIN(dato!F2171:'dato'!F2180)</f>
-        <v>12.451172</v>
-      </c>
-      <c r="F218" s="1">
-        <f>MIN(dato!G2171:'dato'!G2180)</f>
-        <v>-27.709961</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6">
-      <c r="A219" s="1">
-        <f>MIN(dato!B2181:'dato'!B2190)</f>
-        <v>-3.9995120000000002</v>
-      </c>
-      <c r="B219" s="1">
-        <f>MIN(dato!C2181:'dato'!C2190)</f>
-        <v>-2.8305660000000001</v>
-      </c>
-      <c r="C219" s="1">
-        <f>MIN(dato!D2181:'dato'!D2190)</f>
-        <v>1.110962</v>
-      </c>
-      <c r="D219" s="1">
-        <f>MIN(dato!E2181:'dato'!E2190)</f>
-        <v>9.0942380000000007</v>
-      </c>
-      <c r="E219" s="1">
-        <f>MIN(dato!F2181:'dato'!F2190)</f>
-        <v>63.842773000000001</v>
-      </c>
-      <c r="F219" s="1">
-        <f>MIN(dato!G2181:'dato'!G2190)</f>
-        <v>2.868652</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6">
-      <c r="A220" s="1">
-        <f>MIN(dato!B2191:'dato'!B2200)</f>
-        <v>-3.9995120000000002</v>
-      </c>
-      <c r="B220" s="1">
-        <f>MIN(dato!C2191:'dato'!C2200)</f>
-        <v>-0.69677699999999998</v>
-      </c>
-      <c r="C220" s="1">
-        <f>MIN(dato!D2191:'dato'!D2200)</f>
-        <v>-0.73132299999999995</v>
-      </c>
-      <c r="D220" s="1">
-        <f>MIN(dato!E2191:'dato'!E2200)</f>
-        <v>2.2583009999999999</v>
-      </c>
-      <c r="E220" s="1">
-        <f>MIN(dato!F2191:'dato'!F2200)</f>
-        <v>29.724121</v>
-      </c>
-      <c r="F220" s="1">
-        <f>MIN(dato!G2191:'dato'!G2200)</f>
-        <v>82.702636999999996</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6">
-      <c r="A221" s="1">
-        <f>MIN(dato!B2201:'dato'!B2210)</f>
-        <v>9.7778000000000004E-2</v>
-      </c>
-      <c r="B221" s="1">
-        <f>MIN(dato!C2201:'dato'!C2210)</f>
-        <v>0.82324200000000003</v>
-      </c>
-      <c r="C221" s="1">
-        <f>MIN(dato!D2201:'dato'!D2210)</f>
-        <v>-0.27123999999999998</v>
-      </c>
-      <c r="D221" s="1">
-        <f>MIN(dato!E2201:'dato'!E2210)</f>
-        <v>-27.587890999999999</v>
-      </c>
-      <c r="E221" s="1">
-        <f>MIN(dato!F2201:'dato'!F2210)</f>
-        <v>-35.095215000000003</v>
-      </c>
-      <c r="F221" s="1">
-        <f>MIN(dato!G2201:'dato'!G2210)</f>
-        <v>-59.509276999999997</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222" s="1">
-        <f>MIN(dato!B2211:'dato'!B2220)</f>
-        <v>4.6389999999999999E-3</v>
-      </c>
-      <c r="B222" s="1">
-        <f>MIN(dato!C2211:'dato'!C2220)</f>
-        <v>0.98596200000000001</v>
-      </c>
-      <c r="C222" s="1">
-        <f>MIN(dato!D2211:'dato'!D2220)</f>
-        <v>3.6255000000000003E-2</v>
-      </c>
-      <c r="D222" s="1">
-        <f>MIN(dato!E2211:'dato'!E2220)</f>
-        <v>-29.907226999999999</v>
-      </c>
-      <c r="E222" s="1">
-        <f>MIN(dato!F2211:'dato'!F2220)</f>
-        <v>-55.053711</v>
-      </c>
-      <c r="F222" s="1">
-        <f>MIN(dato!G2211:'dato'!G2220)</f>
-        <v>-111.69433600000001</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223" s="1">
-        <f>MIN(dato!B2221:'dato'!B2230)</f>
-        <v>-9.9853999999999998E-2</v>
-      </c>
-      <c r="B223" s="1">
-        <f>MIN(dato!C2221:'dato'!C2230)</f>
-        <v>0.27636699999999997</v>
-      </c>
-      <c r="C223" s="1">
-        <f>MIN(dato!D2221:'dato'!D2230)</f>
-        <v>0.319214</v>
-      </c>
-      <c r="D223" s="1">
-        <f>MIN(dato!E2221:'dato'!E2230)</f>
-        <v>-137.634277</v>
-      </c>
-      <c r="E223" s="1">
-        <f>MIN(dato!F2221:'dato'!F2230)</f>
-        <v>-184.020996</v>
-      </c>
-      <c r="F223" s="1">
-        <f>MIN(dato!G2221:'dato'!G2230)</f>
-        <v>-264.95361300000002</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="A224" s="1">
-        <f>MIN(dato!B2231:'dato'!B2240)</f>
-        <v>-0.75353999999999999</v>
-      </c>
-      <c r="B224" s="1">
-        <f>MIN(dato!C2231:'dato'!C2240)</f>
-        <v>-0.54223600000000005</v>
-      </c>
-      <c r="C224" s="1">
-        <f>MIN(dato!D2231:'dato'!D2240)</f>
-        <v>0.53808599999999995</v>
-      </c>
-      <c r="D224" s="1">
-        <f>MIN(dato!E2231:'dato'!E2240)</f>
-        <v>-125.671387</v>
-      </c>
-      <c r="E224" s="1">
-        <f>MIN(dato!F2231:'dato'!F2240)</f>
-        <v>-213.62304700000001</v>
-      </c>
-      <c r="F224" s="1">
-        <f>MIN(dato!G2231:'dato'!G2240)</f>
-        <v>-283.44726600000001</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="1">
-        <f>MIN(dato!B2241:'dato'!B2250)</f>
-        <v>-0.90454100000000004</v>
-      </c>
-      <c r="B225" s="1">
-        <f>MIN(dato!C2241:'dato'!C2250)</f>
-        <v>-0.26110800000000001</v>
-      </c>
-      <c r="C225" s="1">
-        <f>MIN(dato!D2241:'dato'!D2250)</f>
-        <v>1.1464840000000001</v>
-      </c>
-      <c r="D225" s="1">
-        <f>MIN(dato!E2241:'dato'!E2250)</f>
-        <v>-136.96289100000001</v>
-      </c>
-      <c r="E225" s="1">
-        <f>MIN(dato!F2241:'dato'!F2250)</f>
-        <v>-207.458496</v>
-      </c>
-      <c r="F225" s="1">
-        <f>MIN(dato!G2241:'dato'!G2250)</f>
-        <v>-129.882812</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="1">
-        <f>MIN(dato!B2251:'dato'!B2260)</f>
-        <v>-0.74963400000000002</v>
-      </c>
-      <c r="B226" s="1">
-        <f>MIN(dato!C2251:'dato'!C2260)</f>
-        <v>5.5053999999999999E-2</v>
-      </c>
-      <c r="C226" s="1">
-        <f>MIN(dato!D2251:'dato'!D2260)</f>
-        <v>0.76928700000000005</v>
-      </c>
-      <c r="D226" s="1">
-        <f>MIN(dato!E2251:'dato'!E2260)</f>
-        <v>-10.009766000000001</v>
-      </c>
-      <c r="E226" s="1">
-        <f>MIN(dato!F2251:'dato'!F2260)</f>
-        <v>-98.693848000000003</v>
-      </c>
-      <c r="F226" s="1">
-        <f>MIN(dato!G2251:'dato'!G2260)</f>
-        <v>-62.622070000000001</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6">
-      <c r="A227" s="1">
-        <f>MIN(dato!B2261:'dato'!B2270)</f>
-        <v>-0.72351100000000002</v>
-      </c>
-      <c r="B227" s="1">
-        <f>MIN(dato!C2261:'dato'!C2270)</f>
-        <v>0.252197</v>
-      </c>
-      <c r="C227" s="1">
-        <f>MIN(dato!D2261:'dato'!D2270)</f>
-        <v>0.57739300000000005</v>
-      </c>
-      <c r="D227" s="1">
-        <f>MIN(dato!E2261:'dato'!E2270)</f>
-        <v>9.2773439999999994</v>
-      </c>
-      <c r="E227" s="1">
-        <f>MIN(dato!F2261:'dato'!F2270)</f>
-        <v>-29.663086</v>
-      </c>
-      <c r="F227" s="1">
-        <f>MIN(dato!G2261:'dato'!G2270)</f>
-        <v>-30.700683999999999</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6">
-      <c r="A228" s="1">
-        <f>MIN(dato!B2271:'dato'!B2280)</f>
-        <v>-0.92651399999999995</v>
-      </c>
-      <c r="B228" s="1">
-        <f>MIN(dato!C2271:'dato'!C2280)</f>
-        <v>4.8830000000000002E-3</v>
-      </c>
-      <c r="C228" s="1">
-        <f>MIN(dato!D2271:'dato'!D2280)</f>
-        <v>0.62561</v>
-      </c>
-      <c r="D228" s="1">
-        <f>MIN(dato!E2271:'dato'!E2280)</f>
-        <v>7.1411129999999998</v>
-      </c>
-      <c r="E228" s="1">
-        <f>MIN(dato!F2271:'dato'!F2280)</f>
-        <v>-0.91552699999999998</v>
-      </c>
-      <c r="F228" s="1">
-        <f>MIN(dato!G2271:'dato'!G2280)</f>
-        <v>-13.671875</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6">
-      <c r="A229" s="1">
-        <f>MIN(dato!B2281:'dato'!B2290)</f>
-        <v>-3.9995120000000002</v>
-      </c>
-      <c r="B229" s="1">
-        <f>MIN(dato!C2281:'dato'!C2290)</f>
-        <v>-2.816284</v>
-      </c>
-      <c r="C229" s="1">
-        <f>MIN(dato!D2281:'dato'!D2290)</f>
-        <v>1.656738</v>
-      </c>
-      <c r="D229" s="1">
-        <f>MIN(dato!E2281:'dato'!E2290)</f>
-        <v>-3.4179689999999998</v>
-      </c>
-      <c r="E229" s="1">
-        <f>MIN(dato!F2281:'dato'!F2290)</f>
-        <v>70.190430000000006</v>
-      </c>
-      <c r="F229" s="1">
-        <f>MIN(dato!G2281:'dato'!G2290)</f>
-        <v>28.381347999999999</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6">
-      <c r="A230" s="1">
-        <f>MIN(dato!B2291:'dato'!B2300)</f>
-        <v>-3.9995120000000002</v>
-      </c>
-      <c r="B230" s="1">
-        <f>MIN(dato!C2291:'dato'!C2300)</f>
-        <v>-0.34887699999999999</v>
-      </c>
-      <c r="C230" s="1">
-        <f>MIN(dato!D2291:'dato'!D2300)</f>
-        <v>-0.53515599999999997</v>
-      </c>
-      <c r="D230" s="1">
-        <f>MIN(dato!E2291:'dato'!E2300)</f>
-        <v>116.638184</v>
-      </c>
-      <c r="E230" s="1">
-        <f>MIN(dato!F2291:'dato'!F2300)</f>
-        <v>489.92919899999998</v>
-      </c>
-      <c r="F230" s="1">
-        <f>MIN(dato!G2291:'dato'!G2300)</f>
-        <v>592.10205099999996</v>
       </c>
     </row>
   </sheetData>
@@ -77633,14 +76191,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F230"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F230"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="I222" sqref="I222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1">
@@ -83258,370 +81816,6 @@
         <v>-17.578125</v>
       </c>
     </row>
-    <row r="217" spans="1:6">
-      <c r="A217" s="1">
-        <f>MAX(dato!B2161:'dato'!B2170)</f>
-        <v>-0.61987300000000001</v>
-      </c>
-      <c r="B217" s="1">
-        <f>MAX(dato!C2161:'dato'!C2170)</f>
-        <v>0.29638700000000001</v>
-      </c>
-      <c r="C217" s="1">
-        <f>MAX(dato!D2161:'dato'!D2170)</f>
-        <v>1.146973</v>
-      </c>
-      <c r="D217" s="1">
-        <f>MAX(dato!E2161:'dato'!E2170)</f>
-        <v>19.958496</v>
-      </c>
-      <c r="E217" s="1">
-        <f>MAX(dato!F2161:'dato'!F2170)</f>
-        <v>10.986328</v>
-      </c>
-      <c r="F217" s="1">
-        <f>MAX(dato!G2161:'dato'!G2170)</f>
-        <v>10.559082</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6">
-      <c r="A218" s="1">
-        <f>MAX(dato!B2171:'dato'!B2180)</f>
-        <v>-0.62548800000000004</v>
-      </c>
-      <c r="B218" s="1">
-        <f>MAX(dato!C2171:'dato'!C2180)</f>
-        <v>0.35180699999999998</v>
-      </c>
-      <c r="C218" s="1">
-        <f>MAX(dato!D2171:'dato'!D2180)</f>
-        <v>1.768921</v>
-      </c>
-      <c r="D218" s="1">
-        <f>MAX(dato!E2171:'dato'!E2180)</f>
-        <v>21.728515999999999</v>
-      </c>
-      <c r="E218" s="1">
-        <f>MAX(dato!F2171:'dato'!F2180)</f>
-        <v>43.701172</v>
-      </c>
-      <c r="F218" s="1">
-        <f>MAX(dato!G2171:'dato'!G2180)</f>
-        <v>0.42724600000000001</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6">
-      <c r="A219" s="1">
-        <f>MAX(dato!B2181:'dato'!B2190)</f>
-        <v>-0.977051</v>
-      </c>
-      <c r="B219" s="1">
-        <f>MAX(dato!C2181:'dato'!C2190)</f>
-        <v>0.24231</v>
-      </c>
-      <c r="C219" s="1">
-        <f>MAX(dato!D2181:'dato'!D2190)</f>
-        <v>3.9995120000000002</v>
-      </c>
-      <c r="D219" s="1">
-        <f>MAX(dato!E2181:'dato'!E2190)</f>
-        <v>167.419434</v>
-      </c>
-      <c r="E219" s="1">
-        <f>MAX(dato!F2181:'dato'!F2190)</f>
-        <v>772.399902</v>
-      </c>
-      <c r="F219" s="1">
-        <f>MAX(dato!G2181:'dato'!G2190)</f>
-        <v>648.80371100000002</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6">
-      <c r="A220" s="1">
-        <f>MAX(dato!B2191:'dato'!B2200)</f>
-        <v>-8.0810999999999994E-2</v>
-      </c>
-      <c r="B220" s="1">
-        <f>MAX(dato!C2191:'dato'!C2200)</f>
-        <v>2.6008300000000002</v>
-      </c>
-      <c r="C220" s="1">
-        <f>MAX(dato!D2191:'dato'!D2200)</f>
-        <v>0.53649899999999995</v>
-      </c>
-      <c r="D220" s="1">
-        <f>MAX(dato!E2191:'dato'!E2200)</f>
-        <v>208.557129</v>
-      </c>
-      <c r="E220" s="1">
-        <f>MAX(dato!F2191:'dato'!F2200)</f>
-        <v>581.90917999999999</v>
-      </c>
-      <c r="F220" s="1">
-        <f>MAX(dato!G2191:'dato'!G2200)</f>
-        <v>579.95605499999999</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6">
-      <c r="A221" s="1">
-        <f>MAX(dato!B2201:'dato'!B2210)</f>
-        <v>0.35730000000000001</v>
-      </c>
-      <c r="B221" s="1">
-        <f>MAX(dato!C2201:'dato'!C2210)</f>
-        <v>1.7341310000000001</v>
-      </c>
-      <c r="C221" s="1">
-        <f>MAX(dato!D2201:'dato'!D2210)</f>
-        <v>0.62426800000000005</v>
-      </c>
-      <c r="D221" s="1">
-        <f>MAX(dato!E2201:'dato'!E2210)</f>
-        <v>47.363281000000001</v>
-      </c>
-      <c r="E221" s="1">
-        <f>MAX(dato!F2201:'dato'!F2210)</f>
-        <v>10.314940999999999</v>
-      </c>
-      <c r="F221" s="1">
-        <f>MAX(dato!G2201:'dato'!G2210)</f>
-        <v>44.860840000000003</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222" s="1">
-        <f>MAX(dato!B2211:'dato'!B2220)</f>
-        <v>0.117676</v>
-      </c>
-      <c r="B222" s="1">
-        <f>MAX(dato!C2211:'dato'!C2220)</f>
-        <v>1.0579829999999999</v>
-      </c>
-      <c r="C222" s="1">
-        <f>MAX(dato!D2211:'dato'!D2220)</f>
-        <v>0.44262699999999999</v>
-      </c>
-      <c r="D222" s="1">
-        <f>MAX(dato!E2211:'dato'!E2220)</f>
-        <v>28.930664</v>
-      </c>
-      <c r="E222" s="1">
-        <f>MAX(dato!F2211:'dato'!F2220)</f>
-        <v>0.73242200000000002</v>
-      </c>
-      <c r="F222" s="1">
-        <f>MAX(dato!G2211:'dato'!G2220)</f>
-        <v>-13.793945000000001</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223" s="1">
-        <f>MAX(dato!B2221:'dato'!B2230)</f>
-        <v>8.0569999999999999E-3</v>
-      </c>
-      <c r="B223" s="1">
-        <f>MAX(dato!C2221:'dato'!C2230)</f>
-        <v>1.06958</v>
-      </c>
-      <c r="C223" s="1">
-        <f>MAX(dato!D2221:'dato'!D2230)</f>
-        <v>0.484985</v>
-      </c>
-      <c r="D223" s="1">
-        <f>MAX(dato!E2221:'dato'!E2230)</f>
-        <v>-45.349120999999997</v>
-      </c>
-      <c r="E223" s="1">
-        <f>MAX(dato!F2221:'dato'!F2230)</f>
-        <v>-47.058104999999998</v>
-      </c>
-      <c r="F223" s="1">
-        <f>MAX(dato!G2221:'dato'!G2230)</f>
-        <v>-127.56347700000001</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="A224" s="1">
-        <f>MAX(dato!B2231:'dato'!B2240)</f>
-        <v>-0.15429699999999999</v>
-      </c>
-      <c r="B224" s="1">
-        <f>MAX(dato!C2231:'dato'!C2240)</f>
-        <v>0.23632800000000001</v>
-      </c>
-      <c r="C224" s="1">
-        <f>MAX(dato!D2231:'dato'!D2240)</f>
-        <v>1.117065</v>
-      </c>
-      <c r="D224" s="1">
-        <f>MAX(dato!E2231:'dato'!E2240)</f>
-        <v>-50.78125</v>
-      </c>
-      <c r="E224" s="1">
-        <f>MAX(dato!F2231:'dato'!F2240)</f>
-        <v>-158.81347700000001</v>
-      </c>
-      <c r="F224" s="1">
-        <f>MAX(dato!G2231:'dato'!G2240)</f>
-        <v>-120.72753899999999</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="1">
-        <f>MAX(dato!B2241:'dato'!B2250)</f>
-        <v>-0.72387699999999999</v>
-      </c>
-      <c r="B225" s="1">
-        <f>MAX(dato!C2241:'dato'!C2250)</f>
-        <v>0.17822299999999999</v>
-      </c>
-      <c r="C225" s="1">
-        <f>MAX(dato!D2241:'dato'!D2250)</f>
-        <v>1.631348</v>
-      </c>
-      <c r="D225" s="1">
-        <f>MAX(dato!E2241:'dato'!E2250)</f>
-        <v>-17.51709</v>
-      </c>
-      <c r="E225" s="1">
-        <f>MAX(dato!F2241:'dato'!F2250)</f>
-        <v>-98.266602000000006</v>
-      </c>
-      <c r="F225" s="1">
-        <f>MAX(dato!G2241:'dato'!G2250)</f>
-        <v>-44.799804999999999</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="1">
-        <f>MAX(dato!B2251:'dato'!B2260)</f>
-        <v>-0.62536599999999998</v>
-      </c>
-      <c r="B226" s="1">
-        <f>MAX(dato!C2251:'dato'!C2260)</f>
-        <v>0.246582</v>
-      </c>
-      <c r="C226" s="1">
-        <f>MAX(dato!D2251:'dato'!D2260)</f>
-        <v>1.40564</v>
-      </c>
-      <c r="D226" s="1">
-        <f>MAX(dato!E2251:'dato'!E2260)</f>
-        <v>20.812988000000001</v>
-      </c>
-      <c r="E226" s="1">
-        <f>MAX(dato!F2251:'dato'!F2260)</f>
-        <v>-27.221679999999999</v>
-      </c>
-      <c r="F226" s="1">
-        <f>MAX(dato!G2251:'dato'!G2260)</f>
-        <v>-28.076172</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6">
-      <c r="A227" s="1">
-        <f>MAX(dato!B2261:'dato'!B2270)</f>
-        <v>-0.67260699999999995</v>
-      </c>
-      <c r="B227" s="1">
-        <f>MAX(dato!C2261:'dato'!C2270)</f>
-        <v>0.43457000000000001</v>
-      </c>
-      <c r="C227" s="1">
-        <f>MAX(dato!D2261:'dato'!D2270)</f>
-        <v>0.727661</v>
-      </c>
-      <c r="D227" s="1">
-        <f>MAX(dato!E2261:'dato'!E2270)</f>
-        <v>28.686523000000001</v>
-      </c>
-      <c r="E227" s="1">
-        <f>MAX(dato!F2261:'dato'!F2270)</f>
-        <v>-8.7280270000000009</v>
-      </c>
-      <c r="F227" s="1">
-        <f>MAX(dato!G2261:'dato'!G2270)</f>
-        <v>-13.61084</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6">
-      <c r="A228" s="1">
-        <f>MAX(dato!B2271:'dato'!B2280)</f>
-        <v>-0.60241699999999998</v>
-      </c>
-      <c r="B228" s="1">
-        <f>MAX(dato!C2271:'dato'!C2280)</f>
-        <v>0.41784700000000002</v>
-      </c>
-      <c r="C228" s="1">
-        <f>MAX(dato!D2271:'dato'!D2280)</f>
-        <v>1.397705</v>
-      </c>
-      <c r="D228" s="1">
-        <f>MAX(dato!E2271:'dato'!E2280)</f>
-        <v>16.723633</v>
-      </c>
-      <c r="E228" s="1">
-        <f>MAX(dato!F2271:'dato'!F2280)</f>
-        <v>48.950195000000001</v>
-      </c>
-      <c r="F228" s="1">
-        <f>MAX(dato!G2271:'dato'!G2280)</f>
-        <v>15.136718999999999</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6">
-      <c r="A229" s="1">
-        <f>MAX(dato!B2281:'dato'!B2290)</f>
-        <v>-1.0913090000000001</v>
-      </c>
-      <c r="B229" s="1">
-        <f>MAX(dato!C2281:'dato'!C2290)</f>
-        <v>0.24975600000000001</v>
-      </c>
-      <c r="C229" s="1">
-        <f>MAX(dato!D2281:'dato'!D2290)</f>
-        <v>3.9995120000000002</v>
-      </c>
-      <c r="D229" s="1">
-        <f>MAX(dato!E2281:'dato'!E2290)</f>
-        <v>203.00292999999999</v>
-      </c>
-      <c r="E229" s="1">
-        <f>MAX(dato!F2281:'dato'!F2290)</f>
-        <v>760.25390600000003</v>
-      </c>
-      <c r="F229" s="1">
-        <f>MAX(dato!G2281:'dato'!G2290)</f>
-        <v>669.86084000000005</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6">
-      <c r="A230" s="1">
-        <f>MAX(dato!B2291:'dato'!B2300)</f>
-        <v>-3.9995120000000002</v>
-      </c>
-      <c r="B230" s="1">
-        <f>MAX(dato!C2291:'dato'!C2300)</f>
-        <v>0.56994599999999995</v>
-      </c>
-      <c r="C230" s="1">
-        <f>MAX(dato!D2291:'dato'!D2300)</f>
-        <v>2.3643800000000001</v>
-      </c>
-      <c r="D230" s="1">
-        <f>MAX(dato!E2291:'dato'!E2300)</f>
-        <v>231.933594</v>
-      </c>
-      <c r="E230" s="1">
-        <f>MAX(dato!F2291:'dato'!F2300)</f>
-        <v>817.01660200000003</v>
-      </c>
-      <c r="F230" s="1">
-        <f>MAX(dato!G2291:'dato'!G2300)</f>
-        <v>718.93310499999995</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>